<commit_message>
Tiles are created now using the data from the Excel sheet. Also added variables to the tile class for all relevant data. Reworked the initialisation of the Board to accommodate the changes to the Tile class.
</commit_message>
<xml_diff>
--- a/data/PropertyTycoonBoardData.xlsx
+++ b/data/PropertyTycoonBoardData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kings\Desktop\Sussex\SWE\CWK\TycoonAgileVersion2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor1\Desktop\project files\property-tycoon-38\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2BD454-C31A-44AC-8612-8D761BDE4610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCADFD0-30B1-43A6-AADB-970C2658BE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="770" windowWidth="7550" windowHeight="10030" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
+    <workbookView xWindow="4230" yWindow="3900" windowWidth="21600" windowHeight="11385" xr2:uid="{3AB37EF7-9957-4EAE-A376-EF9CBBC9245A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -679,75 +679,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194933F7-920A-45E1-89BC-1AB0AFB7405E}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>3</v>
+        <v>58</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>58</v>
@@ -755,913 +764,894 @@
       <c r="I4" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
         <v>14</v>
       </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>90</v>
       </c>
       <c r="K6">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="L6">
-        <v>30</v>
-      </c>
-      <c r="M6">
-        <v>90</v>
-      </c>
-      <c r="N6">
-        <v>160</v>
-      </c>
-      <c r="O6">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
         <v>14</v>
       </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
       </c>
       <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
         <v>60</v>
       </c>
-      <c r="I8">
-        <v>4</v>
+      <c r="J8">
+        <v>180</v>
       </c>
       <c r="K8">
-        <v>20</v>
+        <v>320</v>
       </c>
       <c r="L8">
-        <v>60</v>
-      </c>
-      <c r="M8">
-        <v>180</v>
-      </c>
-      <c r="N8">
-        <v>320</v>
-      </c>
-      <c r="O8">
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
         <v>14</v>
       </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
         <v>200</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>82</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>90</v>
+      </c>
+      <c r="J11">
+        <v>270</v>
       </c>
       <c r="K11">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="L11">
-        <v>90</v>
-      </c>
-      <c r="M11">
-        <v>270</v>
-      </c>
-      <c r="N11">
-        <v>400</v>
-      </c>
-      <c r="O11">
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
         <v>14</v>
       </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>90</v>
+      </c>
+      <c r="J13">
+        <v>270</v>
       </c>
       <c r="K13">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="L13">
-        <v>90</v>
-      </c>
-      <c r="M13">
-        <v>270</v>
-      </c>
-      <c r="N13">
-        <v>400</v>
-      </c>
-      <c r="O13">
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
       </c>
       <c r="H14">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="I14">
-        <v>8</v>
+        <v>100</v>
+      </c>
+      <c r="J14">
+        <v>300</v>
       </c>
       <c r="K14">
-        <v>40</v>
+        <v>450</v>
       </c>
       <c r="L14">
-        <v>100</v>
-      </c>
-      <c r="M14">
-        <v>300</v>
-      </c>
-      <c r="N14">
-        <v>450</v>
-      </c>
-      <c r="O14">
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>14</v>
       </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" t="s">
-        <v>17</v>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>140</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
       </c>
       <c r="H16">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="I16">
-        <v>10</v>
+        <v>150</v>
+      </c>
+      <c r="J16">
+        <v>450</v>
       </c>
       <c r="K16">
-        <v>50</v>
+        <v>625</v>
       </c>
       <c r="L16">
-        <v>150</v>
-      </c>
-      <c r="M16">
-        <v>450</v>
-      </c>
-      <c r="N16">
-        <v>625</v>
-      </c>
-      <c r="O16">
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17">
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17">
         <v>150</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="F18" t="s">
-        <v>17</v>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>140</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
       </c>
       <c r="H18">
-        <v>140</v>
+        <v>50</v>
       </c>
       <c r="I18">
-        <v>10</v>
+        <v>150</v>
+      </c>
+      <c r="J18">
+        <v>450</v>
       </c>
       <c r="K18">
-        <v>50</v>
+        <v>625</v>
       </c>
       <c r="L18">
-        <v>150</v>
-      </c>
-      <c r="M18">
-        <v>450</v>
-      </c>
-      <c r="N18">
-        <v>625</v>
-      </c>
-      <c r="O18">
         <v>750</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" t="s">
-        <v>17</v>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>160</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
       </c>
       <c r="H19">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="I19">
-        <v>12</v>
+        <v>180</v>
+      </c>
+      <c r="J19">
+        <v>500</v>
       </c>
       <c r="K19">
-        <v>60</v>
+        <v>700</v>
       </c>
       <c r="L19">
-        <v>180</v>
-      </c>
-      <c r="M19">
-        <v>500</v>
-      </c>
-      <c r="N19">
-        <v>700</v>
-      </c>
-      <c r="O19">
         <v>900</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20">
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20">
         <v>200</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="F21" t="s">
-        <v>17</v>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>180</v>
+      </c>
+      <c r="G21">
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>180</v>
+        <v>70</v>
       </c>
       <c r="I21">
-        <v>14</v>
+        <v>200</v>
+      </c>
+      <c r="J21">
+        <v>550</v>
       </c>
       <c r="K21">
-        <v>70</v>
+        <v>750</v>
       </c>
       <c r="L21">
-        <v>200</v>
-      </c>
-      <c r="M21">
-        <v>550</v>
-      </c>
-      <c r="N21">
-        <v>750</v>
-      </c>
-      <c r="O21">
         <v>950</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
       <c r="E22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" t="s">
         <v>14</v>
       </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>86</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
         <v>35</v>
       </c>
-      <c r="F23" t="s">
-        <v>17</v>
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>180</v>
+      </c>
+      <c r="G23">
+        <v>14</v>
       </c>
       <c r="H23">
-        <v>180</v>
+        <v>70</v>
       </c>
       <c r="I23">
-        <v>14</v>
+        <v>200</v>
+      </c>
+      <c r="J23">
+        <v>550</v>
       </c>
       <c r="K23">
-        <v>70</v>
+        <v>750</v>
       </c>
       <c r="L23">
-        <v>200</v>
-      </c>
-      <c r="M23">
-        <v>550</v>
-      </c>
-      <c r="N23">
-        <v>750</v>
-      </c>
-      <c r="O23">
         <v>950</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="F24" t="s">
-        <v>17</v>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>200</v>
+      </c>
+      <c r="G24">
+        <v>16</v>
       </c>
       <c r="H24">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="I24">
-        <v>16</v>
+        <v>220</v>
+      </c>
+      <c r="J24">
+        <v>600</v>
       </c>
       <c r="K24">
-        <v>80</v>
+        <v>800</v>
       </c>
       <c r="L24">
-        <v>220</v>
-      </c>
-      <c r="M24">
-        <v>600</v>
-      </c>
-      <c r="N24">
-        <v>800</v>
-      </c>
-      <c r="O24">
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
       <c r="E25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" t="s">
         <v>14</v>
       </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="F26" t="s">
-        <v>17</v>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26">
+        <v>220</v>
+      </c>
+      <c r="G26">
+        <v>18</v>
       </c>
       <c r="H26">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="I26">
-        <v>18</v>
+        <v>250</v>
+      </c>
+      <c r="J26">
+        <v>700</v>
       </c>
       <c r="K26">
-        <v>90</v>
+        <v>875</v>
       </c>
       <c r="L26">
-        <v>250</v>
-      </c>
-      <c r="M26">
-        <v>700</v>
-      </c>
-      <c r="N26">
-        <v>875</v>
-      </c>
-      <c r="O26">
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
       <c r="E27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" t="s">
         <v>14</v>
       </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="F28" t="s">
-        <v>17</v>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>220</v>
+      </c>
+      <c r="G28">
+        <v>18</v>
       </c>
       <c r="H28">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="I28">
-        <v>18</v>
+        <v>250</v>
+      </c>
+      <c r="J28">
+        <v>700</v>
       </c>
       <c r="K28">
-        <v>90</v>
+        <v>875</v>
       </c>
       <c r="L28">
-        <v>250</v>
-      </c>
-      <c r="M28">
-        <v>700</v>
-      </c>
-      <c r="N28">
-        <v>875</v>
-      </c>
-      <c r="O28">
         <v>1050</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="F29" t="s">
-        <v>17</v>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>240</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
       </c>
       <c r="H29">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="I29">
-        <v>20</v>
+        <v>300</v>
+      </c>
+      <c r="J29">
+        <v>750</v>
       </c>
       <c r="K29">
-        <v>100</v>
+        <v>925</v>
       </c>
       <c r="L29">
-        <v>300</v>
-      </c>
-      <c r="M29">
-        <v>750</v>
-      </c>
-      <c r="N29">
-        <v>925</v>
-      </c>
-      <c r="O29">
         <v>1100</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>42</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="F30" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
         <v>200</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="G30" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31" t="s">
         <v>43</v>
       </c>
-      <c r="F31" t="s">
-        <v>17</v>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>260</v>
+      </c>
+      <c r="G31">
+        <v>22</v>
       </c>
       <c r="H31">
-        <v>260</v>
+        <v>110</v>
       </c>
       <c r="I31">
-        <v>22</v>
+        <v>330</v>
+      </c>
+      <c r="J31">
+        <v>800</v>
       </c>
       <c r="K31">
-        <v>110</v>
+        <v>975</v>
       </c>
       <c r="L31">
-        <v>330</v>
-      </c>
-      <c r="M31">
-        <v>800</v>
-      </c>
-      <c r="N31">
-        <v>975</v>
-      </c>
-      <c r="O31">
         <v>1150</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="F32" t="s">
-        <v>17</v>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32">
+        <v>260</v>
+      </c>
+      <c r="G32">
+        <v>22</v>
       </c>
       <c r="H32">
-        <v>260</v>
+        <v>110</v>
       </c>
       <c r="I32">
-        <v>22</v>
+        <v>330</v>
+      </c>
+      <c r="J32">
+        <v>800</v>
       </c>
       <c r="K32">
-        <v>110</v>
+        <v>975</v>
       </c>
       <c r="L32">
-        <v>330</v>
-      </c>
-      <c r="M32">
-        <v>800</v>
-      </c>
-      <c r="N32">
-        <v>975</v>
-      </c>
-      <c r="O32">
         <v>1150</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" t="s">
         <v>31</v>
       </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33">
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33">
         <v>150</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34" t="s">
         <v>46</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C34" t="s">
         <v>43</v>
       </c>
-      <c r="F34" t="s">
-        <v>17</v>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34">
+        <v>280</v>
+      </c>
+      <c r="G34">
+        <v>22</v>
       </c>
       <c r="H34">
-        <v>280</v>
+        <v>120</v>
       </c>
       <c r="I34">
-        <v>22</v>
+        <v>360</v>
+      </c>
+      <c r="J34">
+        <v>850</v>
       </c>
       <c r="K34">
-        <v>120</v>
+        <v>1025</v>
       </c>
       <c r="L34">
-        <v>360</v>
-      </c>
-      <c r="M34">
-        <v>850</v>
-      </c>
-      <c r="N34">
-        <v>1025</v>
-      </c>
-      <c r="O34">
         <v>1200</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1671,170 +1661,167 @@
       <c r="D35" t="s">
         <v>48</v>
       </c>
-      <c r="F35" t="s">
+      <c r="E35" t="s">
         <v>14</v>
       </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" t="s">
+      <c r="C36" t="s">
         <v>50</v>
       </c>
-      <c r="F36" t="s">
-        <v>17</v>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <v>300</v>
+      </c>
+      <c r="G36">
+        <v>26</v>
       </c>
       <c r="H36">
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="I36">
-        <v>26</v>
+        <v>390</v>
+      </c>
+      <c r="J36">
+        <v>900</v>
       </c>
       <c r="K36">
-        <v>130</v>
+        <v>1100</v>
       </c>
       <c r="L36">
-        <v>390</v>
-      </c>
-      <c r="M36">
-        <v>900</v>
-      </c>
-      <c r="N36">
-        <v>1100</v>
-      </c>
-      <c r="O36">
         <v>1275</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37" t="s">
         <v>51</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C37" t="s">
         <v>50</v>
       </c>
-      <c r="F37" t="s">
-        <v>17</v>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37">
+        <v>300</v>
+      </c>
+      <c r="G37">
+        <v>26</v>
       </c>
       <c r="H37">
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="I37">
-        <v>26</v>
+        <v>390</v>
+      </c>
+      <c r="J37">
+        <v>900</v>
       </c>
       <c r="K37">
-        <v>130</v>
+        <v>1100</v>
       </c>
       <c r="L37">
-        <v>390</v>
-      </c>
-      <c r="M37">
-        <v>900</v>
-      </c>
-      <c r="N37">
-        <v>1100</v>
-      </c>
-      <c r="O37">
         <v>1275</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
       <c r="E38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" t="s">
         <v>14</v>
       </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C39" t="s">
         <v>50</v>
       </c>
-      <c r="F39" t="s">
-        <v>17</v>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39">
+        <v>320</v>
+      </c>
+      <c r="G39">
+        <v>28</v>
       </c>
       <c r="H39">
-        <v>320</v>
+        <v>150</v>
       </c>
       <c r="I39">
-        <v>28</v>
+        <v>450</v>
+      </c>
+      <c r="J39">
+        <v>1000</v>
       </c>
       <c r="K39">
-        <v>150</v>
+        <v>1200</v>
       </c>
       <c r="L39">
-        <v>450</v>
-      </c>
-      <c r="M39">
-        <v>1000</v>
-      </c>
-      <c r="N39">
-        <v>1200</v>
-      </c>
-      <c r="O39">
         <v>1400</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>90</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
         <v>24</v>
       </c>
-      <c r="F40" t="s">
-        <v>17</v>
-      </c>
-      <c r="H40">
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40">
         <v>200</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -1844,109 +1831,107 @@
       <c r="D41" t="s">
         <v>19</v>
       </c>
-      <c r="F41" t="s">
+      <c r="E41" t="s">
         <v>14</v>
       </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" t="s">
         <v>79</v>
       </c>
-      <c r="F42" t="s">
-        <v>17</v>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>350</v>
+      </c>
+      <c r="G42">
+        <v>35</v>
       </c>
       <c r="H42">
-        <v>350</v>
+        <v>175</v>
       </c>
       <c r="I42">
-        <v>35</v>
+        <v>500</v>
+      </c>
+      <c r="J42">
+        <v>1100</v>
       </c>
       <c r="K42">
-        <v>175</v>
+        <v>1300</v>
       </c>
       <c r="L42">
-        <v>500</v>
-      </c>
-      <c r="M42">
-        <v>1100</v>
-      </c>
-      <c r="N42">
-        <v>1300</v>
-      </c>
-      <c r="O42">
         <v>1500</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>53</v>
       </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
       <c r="E43" t="s">
-        <v>54</v>
-      </c>
-      <c r="F43" t="s">
         <v>14</v>
       </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>55</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" t="s">
         <v>79</v>
       </c>
-      <c r="F44" t="s">
-        <v>17</v>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44">
+        <v>400</v>
+      </c>
+      <c r="G44">
+        <v>50</v>
       </c>
       <c r="H44">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I44">
-        <v>50</v>
+        <v>600</v>
+      </c>
+      <c r="J44">
+        <v>1400</v>
       </c>
       <c r="K44">
-        <v>200</v>
+        <v>1700</v>
       </c>
       <c r="L44">
-        <v>600</v>
-      </c>
-      <c r="M44">
-        <v>1400</v>
-      </c>
-      <c r="N44">
-        <v>1700</v>
-      </c>
-      <c r="O44">
         <v>2000</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>62</v>
       </c>
@@ -1957,7 +1942,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -1972,7 +1957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -1986,7 +1971,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2000,7 +1985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2014,7 +1999,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2028,18 +2013,18 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>